<commit_message>
add 2019 and 2020 corn yields
</commit_message>
<xml_diff>
--- a/data-raw/yields/raw/Marsden 2019 Corn-Soybean Yields.xlsx
+++ b/data-raw/yields/raw/Marsden 2019 Corn-Soybean Yields.xlsx
@@ -1,26 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E63A0D6C-088D-4BCE-B821-6E2B23B07A0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Corn" sheetId="2" r:id="rId1"/>
     <sheet name="Soybean" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -194,7 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -785,43 +778,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -909,7 +902,7 @@
         <v>12.666763239763315</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
@@ -952,7 +945,7 @@
         <v>12.48851543857988</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>16</v>
       </c>
@@ -999,7 +992,7 @@
         <v>13.123293159763314</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
@@ -1042,7 +1035,7 @@
         <v>12.485268207337276</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>19</v>
       </c>
@@ -1089,7 +1082,7 @@
         <v>13.130585433372783</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
@@ -1132,7 +1125,7 @@
         <v>13.296726100828399</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>21</v>
       </c>
@@ -1179,7 +1172,7 @@
         <v>12.474238818461536</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="1" t="s">
@@ -1222,7 +1215,7 @@
         <v>12.969889476923079</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>25</v>
       </c>
@@ -1269,7 +1262,7 @@
         <v>12.249116114556214</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
@@ -1312,7 +1305,7 @@
         <v>11.844415924260353</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>27</v>
       </c>
@@ -1359,7 +1352,7 @@
         <v>11.702181597159761</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="1" t="s">
@@ -1402,7 +1395,7 @@
         <v>12.65668562556213</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>31</v>
       </c>
@@ -1449,7 +1442,7 @@
         <v>12.697681919999999</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="1" t="s">
@@ -1492,7 +1485,7 @@
         <v>12.798514048757395</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>33</v>
       </c>
@@ -1539,7 +1532,7 @@
         <v>12.268263581538461</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
@@ -1582,7 +1575,7 @@
         <v>12.272924478106509</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>35</v>
       </c>
@@ -1629,7 +1622,7 @@
         <v>13.67935351668639</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="1" t="s">
@@ -1672,7 +1665,7 @@
         <v>13.447176482840236</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42</v>
       </c>
@@ -1719,7 +1712,7 @@
         <v>12.094144802840235</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="1" t="s">
@@ -1762,7 +1755,7 @@
         <v>12.655719854201184</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43</v>
       </c>
@@ -1809,7 +1802,7 @@
         <v>12.787442669822484</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
@@ -1852,7 +1845,7 @@
         <v>12.780374343195268</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45</v>
       </c>
@@ -1899,7 +1892,7 @@
         <v>12.654586122603549</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="1" t="s">
@@ -1942,7 +1935,7 @@
         <v>13.241565159763313</v>
       </c>
     </row>
-    <row r="33" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L33" s="18" t="s">
         <v>18</v>
       </c>
@@ -1957,7 +1950,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K34" s="21" t="s">
         <v>20</v>
       </c>
@@ -1981,7 +1974,7 @@
         <v>0.4191879715555798</v>
       </c>
     </row>
-    <row r="35" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K35" s="23" t="s">
         <v>21</v>
       </c>
@@ -2005,7 +1998,7 @@
         <v>0.1734794499111541</v>
       </c>
     </row>
-    <row r="36" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K36" s="23" t="s">
         <v>22</v>
       </c>
@@ -2029,7 +2022,7 @@
         <v>0.23314460411789986</v>
       </c>
     </row>
-    <row r="37" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K37" s="23" t="s">
         <v>23</v>
       </c>
@@ -2053,7 +2046,7 @@
         <v>0.17519044514728438</v>
       </c>
     </row>
-    <row r="38" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K38" s="23" t="s">
         <v>24</v>
       </c>
@@ -2077,7 +2070,7 @@
         <v>6.5933300698149025E-2</v>
       </c>
     </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K39" s="23" t="s">
         <v>25</v>
       </c>
@@ -2101,7 +2094,7 @@
         <v>9.9855760090372364E-2</v>
       </c>
     </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K40" s="25"/>
       <c r="L40" s="9"/>
       <c r="M40" s="26"/>
@@ -2109,7 +2102,7 @@
       <c r="O40" s="35"/>
       <c r="P40" s="36"/>
     </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K41" s="23" t="s">
         <v>13</v>
       </c>
@@ -2133,7 +2126,7 @@
         <v>0.22115100758653375</v>
       </c>
     </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K42" s="23" t="s">
         <v>16</v>
       </c>
@@ -2157,7 +2150,7 @@
         <v>0.13678657501000119</v>
       </c>
     </row>
-    <row r="43" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K43" s="23" t="s">
         <v>17</v>
       </c>
@@ -2181,7 +2174,7 @@
         <v>5.8666476636059922E-2</v>
       </c>
     </row>
-    <row r="44" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K44" s="25"/>
       <c r="L44" s="9"/>
       <c r="M44" s="36"/>
@@ -2189,7 +2182,7 @@
       <c r="O44" s="35"/>
       <c r="P44" s="36"/>
     </row>
-    <row r="45" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K45" s="23" t="s">
         <v>26</v>
       </c>
@@ -2213,7 +2206,7 @@
         <v>0.15279648755926536</v>
       </c>
     </row>
-    <row r="46" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K46" s="27" t="s">
         <v>15</v>
       </c>
@@ -2244,56 +2237,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P47"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
@@ -2334,7 +2327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>13</v>
       </c>
@@ -2381,7 +2374,7 @@
         <v>3.578879170540012</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>13</v>
       </c>
@@ -2428,7 +2421,7 @@
         <v>3.5710833759271292</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2475,7 +2468,7 @@
         <v>4.0532101038386461</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>15</v>
       </c>
@@ -2522,7 +2515,7 @@
         <v>4.0175442729472985</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>18</v>
       </c>
@@ -2569,7 +2562,7 @@
         <v>4.0247983402472336</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>18</v>
       </c>
@@ -2616,7 +2609,7 @@
         <v>4.0465605421470388</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>24</v>
       </c>
@@ -2663,7 +2656,7 @@
         <v>3.685734883018867</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>24</v>
       </c>
@@ -2710,7 +2703,7 @@
         <v>3.6797674180871822</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>26</v>
       </c>
@@ -2757,7 +2750,7 @@
         <v>3.8908887093298627</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>26</v>
       </c>
@@ -2804,7 +2797,7 @@
         <v>3.8573947253090433</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>28</v>
       </c>
@@ -2851,7 +2844,7 @@
         <v>4.3866002371372801</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>28</v>
       </c>
@@ -2898,7 +2891,7 @@
         <v>4.1818597600520482</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>34</v>
       </c>
@@ -2945,7 +2938,7 @@
         <v>3.858114206896551</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>34</v>
       </c>
@@ -2992,7 +2985,7 @@
         <v>3.6245281611450868</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>36</v>
       </c>
@@ -3039,7 +3032,7 @@
         <v>3.8200874888744294</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>36</v>
       </c>
@@ -3086,7 +3079,7 @@
         <v>3.7695474342225106</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>37</v>
       </c>
@@ -3133,7 +3126,7 @@
         <v>4.1856391545087819</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>37</v>
       </c>
@@ -3180,7 +3173,7 @@
         <v>4.2196607583604413</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44</v>
       </c>
@@ -3227,7 +3220,7 @@
         <v>3.6865164375276498</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>44</v>
       </c>
@@ -3274,7 +3267,7 @@
         <v>3.8038511877163295</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
@@ -3321,7 +3314,7 @@
         <v>4.4019051623266101</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>46</v>
       </c>
@@ -3368,7 +3361,7 @@
         <v>4.3121663400390364</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>47</v>
       </c>
@@ -3415,7 +3408,7 @@
         <v>4.1588970114248527</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>47</v>
       </c>
@@ -3462,7 +3455,7 @@
         <v>4.1662385451138579</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L34" s="18" t="s">
         <v>18</v>
       </c>
@@ -3476,7 +3469,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K35" s="21" t="s">
         <v>34</v>
       </c>
@@ -3500,7 +3493,7 @@
         <v>5.7759769491714873E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -3527,7 +3520,7 @@
         <v>4.9886188290602006E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -3554,7 +3547,7 @@
         <v>7.6851760245893463E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K38" s="23" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3571,7 @@
         <v>8.7764574435965151E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K39" s="23" t="s">
         <v>38</v>
       </c>
@@ -3602,7 +3595,7 @@
         <v>8.9718369424838976E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K40" s="23" t="s">
         <v>39</v>
       </c>
@@ -3626,7 +3619,7 @@
         <v>5.5110118171747435E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K41" s="25"/>
       <c r="L41" s="9"/>
       <c r="M41" s="26"/>
@@ -3634,7 +3627,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="33"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K42" s="23" t="s">
         <v>33</v>
       </c>
@@ -3658,7 +3651,7 @@
         <v>3.6223624695045552E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K43" s="23" t="s">
         <v>32</v>
       </c>
@@ -3682,7 +3675,7 @@
         <v>5.4812796368995338E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K44" s="23" t="s">
         <v>31</v>
       </c>
@@ -3706,7 +3699,7 @@
         <v>5.0536493752599478E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K45" s="25"/>
       <c r="L45" s="9"/>
       <c r="M45" s="26"/>
@@ -3714,7 +3707,7 @@
       <c r="O45" s="9"/>
       <c r="P45" s="33"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K46" s="23" t="s">
         <v>26</v>
       </c>
@@ -3738,7 +3731,7 @@
         <v>7.7383396615228084E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K47" s="27" t="s">
         <v>15</v>
       </c>

</xml_diff>